<commit_message>
rework ids with ips
</commit_message>
<xml_diff>
--- a/ePICreator/Calcio_Vitamina D.xlsx
+++ b/ePICreator/Calcio_Vitamina D.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CF5F34-181B-FE43-9417-F7F7963C37E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F12161-BD46-324F-9354-F0788B751936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AdministrableProductDefinition" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>concept</t>
-  </si>
-  <si>
-    <t>title</t>
   </si>
   <si>
     <t>role</t>
@@ -586,9 +583,6 @@
     </r>
   </si>
   <si>
-    <t>TEST PURPOSES ONLY -CALCIO/VITAMINA D3 ROVI 1000 mg/880 UI COMPRIMIDOS EFERVESCENTES</t>
-  </si>
-  <si>
     <t>&lt;div xmlns='http://www.w3.org/1999/xhtml'&gt; 
 &lt;p&gt;&lt;strong&gt;Prospecto: informaci&amp;oacute;n para el usuario&lt;/strong&gt;&lt;/p&gt;
 &lt;p&gt;&amp;nbsp;&lt;/p&gt;
@@ -819,12 +813,18 @@
   <si>
     <t>es</t>
   </si>
+  <si>
+    <t>https://cima.aemps.es/ids|https://www.who-umc.org/phpid</t>
+  </si>
+  <si>
+    <t>68290|0xF79CABF272B6A7EEF104DDDA44E82716</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -948,6 +948,14 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -966,10 +974,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -995,8 +1004,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1345,25 +1356,25 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>6</v>
       </c>
       <c r="J1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -1371,16 +1382,16 @@
     </row>
     <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F2" s="18">
         <v>100000073681</v>
@@ -1444,31 +1455,31 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" t="s">
-        <v>84</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" t="s">
         <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L1" t="s">
-        <v>82</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -1476,13 +1487,13 @@
     </row>
     <row r="2" spans="1:14" ht="18" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" t="s">
-        <v>117</v>
-      </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1491,19 +1502,19 @@
         <v>100.09</v>
       </c>
       <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
-        <v>152</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="K2" t="s">
-        <v>45</v>
-      </c>
       <c r="L2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -1536,13 +1547,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1553,16 +1564,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1593,7 +1604,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>13</v>
@@ -1605,7 +1616,7 @@
         <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
         <v>12</v>
@@ -1633,49 +1644,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="48.6640625" customWidth="1"/>
-    <col min="5" max="5" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="15" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>87</v>
       </c>
       <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
         <v>88</v>
-      </c>
-      <c r="I1" t="s">
-        <v>87</v>
       </c>
       <c r="J1" t="s">
         <v>89</v>
@@ -1696,56 +1706,50 @@
         <v>94</v>
       </c>
       <c r="P1" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="C2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="N2" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="O2" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1787,31 +1791,31 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
       <c r="G1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
       </c>
       <c r="I1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -1820,10 +1824,10 @@
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>117</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -1832,10 +1836,10 @@
         <v>72072</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>8</v>
@@ -1844,16 +1848,16 @@
         <v>2500</v>
       </c>
       <c r="L2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" t="s">
-        <v>120</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -1862,10 +1866,10 @@
         <v>72072</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H3" s="5" t="s">
         <v>8</v>
@@ -1874,16 +1878,16 @@
         <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
-      </c>
-      <c r="C4" t="s">
-        <v>122</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
@@ -1892,27 +1896,27 @@
         <v>72072</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
@@ -1921,10 +1925,10 @@
         <v>72072</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>8</v>
@@ -1933,15 +1937,15 @@
         <v>396.44</v>
       </c>
       <c r="L5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C6" t="s">
         <v>125</v>
-      </c>
-      <c r="C6" t="s">
-        <v>126</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
@@ -1950,10 +1954,10 @@
         <v>72072</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H6" s="5" t="s">
         <v>8</v>
@@ -1962,15 +1966,15 @@
         <v>3.68</v>
       </c>
       <c r="L6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -1979,10 +1983,10 @@
         <v>72072</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>8</v>
@@ -1991,18 +1995,18 @@
         <v>0.73</v>
       </c>
       <c r="L7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" t="s">
         <v>127</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>128</v>
-      </c>
-      <c r="D8" t="s">
-        <v>129</v>
       </c>
       <c r="E8">
         <v>100000072082</v>
@@ -2013,13 +2017,13 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
         <v>130</v>
       </c>
-      <c r="C9" t="s">
-        <v>131</v>
-      </c>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9">
         <v>100000072082</v>
@@ -2030,13 +2034,13 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10">
         <v>100000072082</v>
@@ -2047,13 +2051,13 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" t="s">
         <v>133</v>
       </c>
-      <c r="C11" t="s">
-        <v>134</v>
-      </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E11">
         <v>100000072082</v>
@@ -2064,13 +2068,13 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
         <v>135</v>
       </c>
-      <c r="C12" t="s">
-        <v>136</v>
-      </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E12">
         <v>100000072082</v>
@@ -2081,13 +2085,13 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" t="s">
         <v>137</v>
       </c>
-      <c r="C13" t="s">
-        <v>138</v>
-      </c>
       <c r="D13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E13">
         <v>100000072082</v>
@@ -2136,13 +2140,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I1" t="s">
         <v>12</v>
@@ -2150,7 +2154,7 @@
     </row>
     <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B2" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C2">
         <v>68290</v>
@@ -2159,7 +2163,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F2" s="18">
         <v>100000073681</v>
@@ -2179,133 +2183,142 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.33203125" customWidth="1"/>
-    <col min="14" max="14" width="11" customWidth="1"/>
+    <col min="3" max="4" width="27.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.33203125" customWidth="1"/>
+    <col min="15" max="15" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+      <c r="T1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
         <v>96</v>
       </c>
-      <c r="K1" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="O1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>99</v>
-      </c>
-      <c r="R1" t="s">
-        <v>100</v>
-      </c>
-      <c r="S1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>100000000000</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A169F2A9-AF95-BF4C-84C7-D772931B0CAD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -2341,25 +2354,25 @@
         <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" t="s">
         <v>70</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>72</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
-        <v>74</v>
-      </c>
       <c r="L1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M1" t="s">
         <v>12</v>
@@ -2367,34 +2380,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
       </c>
       <c r="F2" s="7">
         <v>220000000034</v>
       </c>
       <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" t="s">
-        <v>34</v>
-      </c>
       <c r="I2" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" t="s">
         <v>103</v>
-      </c>
-      <c r="K2" t="s">
-        <v>104</v>
       </c>
       <c r="L2" s="15">
         <v>28037</v>
@@ -2447,58 +2460,58 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" t="s">
         <v>76</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="L1" t="s">
-        <v>114</v>
-      </c>
-      <c r="M1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" t="s">
-        <v>78</v>
-      </c>
       <c r="O1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q1" t="s">
+        <v>107</v>
+      </c>
+      <c r="R1" t="s">
         <v>108</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>109</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>110</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>111</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>112</v>
-      </c>
-      <c r="V1" t="s">
-        <v>113</v>
       </c>
       <c r="W1" t="s">
         <v>12</v>
@@ -2506,31 +2519,31 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>37</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F2" t="s">
-        <v>38</v>
       </c>
       <c r="G2">
         <v>100000155527</v>
       </c>
       <c r="H2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I2">
         <v>123456</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K2">
         <v>100000073496</v>
@@ -2539,13 +2552,13 @@
         <v>30</v>
       </c>
       <c r="M2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="P2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2559,7 +2572,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2581,22 +2594,22 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
@@ -2605,31 +2618,31 @@
     <row r="2" spans="1:11" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C2" s="11">
         <v>68290</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H2" s="2">
         <v>100000072062</v>
       </c>
       <c r="I2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" x14ac:dyDescent="0.2">

</xml_diff>